<commit_message>
Project : Decision edit
</commit_message>
<xml_diff>
--- a/phonegap project.xlsx
+++ b/phonegap project.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="temp note" sheetId="2" r:id="rId1"/>
@@ -12,9 +17,9 @@
     <sheet name="exercise" sheetId="1" r:id="rId3"/>
     <sheet name="decision" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>clock centerlize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -339,10 +344,6 @@
   </si>
   <si>
     <t>True: 在開場畫面出現時，顯示iOS Loading圖樣</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>change to localstorage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -364,47 +365,109 @@
     <t>http://www.w3schools.com/html/html5_webstorage.asp</t>
   </si>
   <si>
-    <t>localstorage["bar"] = "hello";</t>
+    <t>if(window.localStorage){</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alert('This browser supports localStorage');</t>
+  </si>
+  <si>
+    <t>}else{</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alert('This browser does NOT support localStorage');</t>
+  </si>
+  <si>
+    <t>external links should open in the default browser, 'true' would use the webview the app lives in</t>
+  </si>
+  <si>
+    <t>&lt;preference name="target-device" value="universal" /&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>possible values handset, tablet, or universal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB change to localstorage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open list : SESSION change to ??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$num_last_record = 5;</t>
+  </si>
+  <si>
+    <t>$max_width_list = 5;</t>
+  </si>
+  <si>
+    <t>constant to localstorage?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設定資料</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>設定資料</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>取得資料</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">var foo = localstorage,getItem("bar"); </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>更新</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>取得資料</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>移除</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>localstorage.setItem("bar", "hello JSDC!");</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清除所有資料</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">localstorage.removeItem("bar"); </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>移除</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">localstorage.clear(); </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>清除所有資料</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(window.localStorage){</t>
   </si>
   <si>
     <r>
@@ -424,19 +487,6 @@
       </rPr>
       <t>localstorage</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> alert('This browser supports localStorage');</t>
-  </si>
-  <si>
-    <t>}else{</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> alert('This browser does NOT support localStorage');</t>
-  </si>
-  <si>
-    <t>var b = localStorage.getItem("b");</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -469,25 +519,96 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>external links should open in the default browser, 'true' would use the webview the app lives in</t>
-  </si>
-  <si>
-    <t>&lt;preference name="target-device" value="universal" /&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>possible values handset, tablet, or universal</t>
+    <t>openlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Button function redesign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8009/app/decision/www/app_decision.php</t>
+  </si>
+  <si>
+    <t>hyperlink function in app?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page change for jqm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; sample for test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>form submit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title add decision_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>localStorage["bar"] = "hello";</t>
+  </si>
+  <si>
+    <t>localStorage.setItem("bar", "hello JSDC!");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">localStorage.clear(); </t>
+  </si>
+  <si>
+    <t>var b = localStorage.getItem("b");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var foo = localStorage,getItem("bar"); </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>when draw_code change -&gt; update DRAW content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>how to change to draw page? -&gt; test on APP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purge -&gt; add comfirm msg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add !! between selection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="_-[$€]* #,##0.00_-;\-[$€]* #,##0.00_-;_-[$€]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -556,13 +677,31 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -579,7 +718,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -607,8 +746,20 @@
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,6 +767,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -882,28 +1038,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C40" sqref="C40:D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.6640625" customWidth="1"/>
-    <col min="4" max="4" width="111.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.6328125" customWidth="1"/>
+    <col min="4" max="4" width="111.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -911,7 +1067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -919,7 +1075,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -930,7 +1086,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -938,7 +1094,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -949,7 +1105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -960,7 +1116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -971,7 +1127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>25</v>
       </c>
@@ -979,7 +1135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
         <v>27</v>
       </c>
@@ -987,7 +1143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
         <v>29</v>
       </c>
@@ -995,7 +1151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -1003,7 +1159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -1011,7 +1167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
         <v>33</v>
       </c>
@@ -1019,7 +1175,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
         <v>35</v>
       </c>
@@ -1027,7 +1183,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
         <v>37</v>
       </c>
@@ -1035,7 +1191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
         <v>41</v>
       </c>
@@ -1043,7 +1199,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
         <v>42</v>
       </c>
@@ -1051,7 +1207,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
         <v>51</v>
       </c>
@@ -1059,7 +1215,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
         <v>53</v>
       </c>
@@ -1067,7 +1223,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="32.4">
+    <row r="20" spans="3:4" ht="34" x14ac:dyDescent="0.4">
       <c r="C20" s="5" t="s">
         <v>55</v>
       </c>
@@ -1075,7 +1231,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C21" s="5" t="s">
         <v>57</v>
       </c>
@@ -1083,7 +1239,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
         <v>59</v>
       </c>
@@ -1091,7 +1247,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
         <v>43</v>
       </c>
@@ -1099,7 +1255,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:4">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C24" t="s">
         <v>65</v>
       </c>
@@ -1107,7 +1263,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C25" t="s">
         <v>67</v>
       </c>
@@ -1115,7 +1271,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="3:4">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
         <v>69</v>
       </c>
@@ -1123,7 +1279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="3:4">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C27" t="s">
         <v>71</v>
       </c>
@@ -1131,7 +1287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
         <v>73</v>
       </c>
@@ -1139,7 +1295,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C29" s="4" t="s">
         <v>77</v>
       </c>
@@ -1147,7 +1303,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C30" s="4" t="s">
         <v>76</v>
       </c>
@@ -1155,12 +1311,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
         <v>80</v>
       </c>
@@ -1168,7 +1324,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
         <v>81</v>
       </c>
@@ -1176,23 +1332,23 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="3:4">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
         <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C35" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C40" t="s">
         <v>60</v>
       </c>
@@ -1200,7 +1356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="3:4">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C41" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="3:4">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.4">
       <c r="D42" t="s">
         <v>39</v>
       </c>
@@ -1220,7 +1376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -1230,17 +1386,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1252,22 +1408,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="1.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1275,7 +1431,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1283,7 +1439,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
@@ -1291,7 +1447,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1304,104 +1460,196 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C7" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="C2" s="8" t="s">
+      <c r="D7" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3" s="8" t="s">
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="C5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="C6" s="8" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A35" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="9" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" s="9" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
> decision : update list function
</commit_message>
<xml_diff>
--- a/phonegap project.xlsx
+++ b/phonegap project.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>clock centerlize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -541,12 +541,6 @@
     <t>localStorage["bar"] = "hello";</t>
   </si>
   <si>
-    <t>localStorage.setItem("bar", "hello JSDC!");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
-  </si>
-  <si>
     <t xml:space="preserve">localStorage.clear(); </t>
   </si>
   <si>
@@ -569,19 +563,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>purge -&gt; add comfirm msg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>add !! between selection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select list from localStorage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>myfavor -&gt; another item to storage myfavor group?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -612,26 +594,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>edit title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete selection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>start draw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add selection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>default setting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -644,15 +606,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>create list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select number &amp; content of localstorage title by decision_%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> -&gt; select all localstorage -&gt; filter by preg -&gt; save result to array</t>
+    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>localStorage.setItem("bar", "hello JSDC!");</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load default open for editing list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; open dialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete_selection(title,selection)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete_group(title)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_myfavor(title)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; another item to storage myfavor group?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>navigator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_selection(title)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input : new_title_titlename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to refresh page to get new localstorage data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; add confirm msg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; add comfirm msg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -663,7 +677,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="_-[$€]* #,##0.00_-;\-[$€]* #,##0.00_-;_-[$€]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -738,6 +752,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -754,7 +774,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFF8585"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,7 +793,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -813,17 +833,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,6 +856,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF8585"/>
       <color rgb="FFFF3300"/>
     </mruColors>
   </colors>
@@ -1102,7 +1126,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1225,7 +1249,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1236,7 +1260,7 @@
     </row>
     <row r="13" spans="1:4" ht="64.8">
       <c r="A13" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -1247,7 +1271,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -1482,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6"/>
@@ -1498,7 +1522,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>106</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -1524,7 +1548,7 @@
         <v>111</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>98</v>
@@ -1532,10 +1556,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>99</v>
@@ -1543,7 +1567,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="C5" s="8" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>100</v>
@@ -1551,7 +1575,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="C6" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>101</v>
@@ -1597,133 +1621,134 @@
         <v>109</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="9" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="13"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="12" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="9"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="12" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="13"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="9" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="9" t="s">
+    <row r="51" spans="1:1">
+      <c r="A51" s="9" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1798,10 +1823,10 @@
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
> add array sorting to unify order > adjust alert msg format > add custom confirm dialog > update default open list rule
</commit_message>
<xml_diff>
--- a/phonegap project.xlsx
+++ b/phonegap project.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
   <si>
     <t>clock centerlize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -386,16 +386,6 @@
   <si>
     <t>DB change to localstorage</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>open list : SESSION change to ??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$num_last_record = 5;</t>
-  </si>
-  <si>
-    <t>$max_width_list = 5;</t>
   </si>
   <si>
     <r>
@@ -507,10 +497,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>openlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Button function redesign</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -570,15 +556,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>constant by javascript</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>constants.constant1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>draw code -&gt; set to localstorage to keep draw list?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -657,6 +635,17 @@
   </si>
   <si>
     <t xml:space="preserve">localStorage.removeItem("bar"); </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/5747382/jquery-mobile-alert-confirmation-dialogs</t>
+  </si>
+  <si>
+    <t>jQuery mobile confirm dialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom confirm msg can't reload page after confirm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -667,7 +656,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="_-[$€]* #,##0.00_-;\-[$€]* #,##0.00_-;_-[$€]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -764,6 +753,12 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -799,7 +794,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -862,6 +857,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,7 +1139,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1152,7 +1150,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A25"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1264,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>12</v>
@@ -1277,7 +1275,7 @@
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>33</v>
@@ -1288,7 +1286,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>35</v>
@@ -1307,7 +1305,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>41</v>
@@ -1318,7 +1316,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>42</v>
@@ -1329,7 +1327,7 @@
     </row>
     <row r="18" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>51</v>
@@ -1371,6 +1369,9 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="C23" s="15" t="s">
         <v>43</v>
       </c>
@@ -1379,6 +1380,9 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>136</v>
+      </c>
       <c r="C24" s="15" t="s">
         <v>65</v>
       </c>
@@ -1532,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1553,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>84</v>
@@ -1563,64 +1567,64 @@
         <v>93</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>87</v>
@@ -1629,7 +1633,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>88</v>
@@ -1638,7 +1642,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>89</v>
@@ -1647,108 +1651,80 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1822,10 +1798,10 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
> decision : use refresh list replace reload()
</commit_message>
<xml_diff>
--- a/phonegap project.xlsx
+++ b/phonegap project.xlsx
@@ -10,8 +10,10 @@
     <sheet name="temp note" sheetId="2" r:id="rId1"/>
     <sheet name="APP idea" sheetId="3" r:id="rId2"/>
     <sheet name="decision" sheetId="4" r:id="rId3"/>
-    <sheet name="close -&gt;" sheetId="5" r:id="rId4"/>
-    <sheet name="exercise" sheetId="1" r:id="rId5"/>
+    <sheet name="scoreboard" sheetId="6" r:id="rId4"/>
+    <sheet name="vocabolary" sheetId="7" r:id="rId5"/>
+    <sheet name="close -&gt;" sheetId="5" r:id="rId6"/>
+    <sheet name="exercise" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="149">
   <si>
     <t>clock centerlize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -381,10 +383,6 @@
   </si>
   <si>
     <t>possible values handset, tablet, or universal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB change to localstorage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -497,25 +495,13 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Button function redesign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://localhost:8009/app/decision/www/app_decision.php</t>
   </si>
   <si>
-    <t>page change for jqm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>form submit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>title add decision_</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>localStorage["bar"] = "hello";</t>
   </si>
   <si>
@@ -538,10 +524,6 @@
   </si>
   <si>
     <t>Set</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add !! between selection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -568,14 +550,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>delete_selection(title,selection)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete_group(title)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>add_myfavor(title)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -584,22 +558,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>navigator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> -&gt; add confirm msg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>purge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> -&gt; add comfirm msg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>localStorage.setItem("bar", "hello JSDC!");</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -618,10 +576,6 @@
   <si>
     <t>test on app</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>arrayObject.splice(index,howmany,item1,.....,itemX)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>javascript</t>
@@ -641,18 +595,6 @@
     <t>http://stackoverflow.com/questions/5747382/jquery-mobile-alert-confirmation-dialogs</t>
   </si>
   <si>
-    <t>jQuery mobile confirm dialog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>custom confirm msg can't reload page after confirm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> =&gt; try refresh list function -&gt; style error and need to prevent duplicate data about group title rename</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>var arr = reallyLongArray;</t>
   </si>
   <si>
@@ -671,11 +613,74 @@
     <t>$('table').append(textToInsert);</t>
   </si>
   <si>
-    <t>jQuery each</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create list -&gt; use refresh draw content to replace reload(), for better ux?</t>
+    <t>create more drawing method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drawing method select : random/..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page change on jqm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.trigger( "create" );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">jQuery </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>each</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add trigger after append to load jQuery mobile style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jQuery mobile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>confirm dialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update to jQuery mobile style?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate style.css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use localstorage replace mysql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; delete element itself</t>
+  </si>
+  <si>
+    <t>arrayObject.splice(index,howmany,item1,.....,itemX)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>splice()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check localstorage clear rule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purge =&gt; change to only remove decision data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -762,13 +767,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
@@ -789,8 +787,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,12 +805,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,7 +823,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -849,46 +848,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1169,7 +1159,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1177,19 +1167,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF8585"/>
+  </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="15"/>
-    <col min="3" max="3" width="54.625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="111.5" style="15" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="15"/>
+    <col min="1" max="1" width="47.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="10"/>
+    <col min="3" max="3" width="54.625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="111.5" style="10" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1201,349 +1194,374 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="A17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="15" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
+    <row r="19" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
+      <c r="A20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="17" t="s">
+      <c r="A21" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="C27" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="15" t="s">
+      <c r="A32" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="A33" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="10" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="A34" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="15" t="s">
+      <c r="A35" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="10" t="s">
         <v>92</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1562,7 +1580,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1588,24 +1606,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>102</v>
+      <c r="A1" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>84</v>
@@ -1615,68 +1633,69 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>131</v>
+      <c r="A7" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>129</v>
+      <c r="A8" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>87</v>
@@ -1684,8 +1703,8 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>103</v>
+      <c r="A9" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>88</v>
@@ -1693,100 +1712,95 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>104</v>
-      </c>
       <c r="C10" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>130</v>
-      </c>
       <c r="C11" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>147</v>
+      <c r="B16" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1795,7 +1809,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
@@ -1813,7 +1852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C7"/>
   <sheetViews>
@@ -1860,10 +1899,10 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
> decision : purge localstorage select only for this program
</commit_message>
<xml_diff>
--- a/phonegap project.xlsx
+++ b/phonegap project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="temp note" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
   <si>
     <t>clock centerlize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -588,10 +588,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://stackoverflow.com/questions/5747382/jquery-mobile-alert-confirmation-dialogs</t>
   </si>
   <si>
@@ -680,10 +676,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>purge =&gt; change to only remove decision data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LIST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -716,15 +708,38 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>oahehc_scoreboard_test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>allen!!-50!50!!200</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>andrew!!100!-50!!80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oahehc_scoreboard_test_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oahehc_scoreboard_test_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show title, expand to list player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>how to prevent data been delete by other program =&gt; study phonegap DB plugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.toright.com/posts/2356/android-webapp-%E9%96%8B%E7%99%BC%E6%95%99%E5%AD%B8-html5-web-storage.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; use JSON for data?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1213,7 +1228,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1393,7 +1408,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>42</v>
@@ -1404,7 +1419,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>51</v>
@@ -1426,7 +1441,7 @@
     </row>
     <row r="20" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>55</v>
@@ -1437,7 +1452,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>57</v>
@@ -1456,7 +1471,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>43</v>
@@ -1467,7 +1482,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>65</v>
@@ -1478,7 +1493,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>67</v>
@@ -1489,7 +1504,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>69</v>
@@ -1500,7 +1515,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>71</v>
@@ -1527,7 +1542,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>76</v>
@@ -1538,7 +1553,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>79</v>
@@ -1546,7 +1561,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>80</v>
@@ -1557,7 +1572,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>81</v>
@@ -1568,7 +1583,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>52</v>
@@ -1579,7 +1594,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>91</v>
@@ -1590,12 +1605,12 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1734,7 @@
         <v>118</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>96</v>
@@ -1727,7 +1742,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>103</v>
@@ -1758,7 +1773,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>88</v>
@@ -1802,7 +1817,7 @@
         <v>107</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1810,12 +1825,7 @@
         <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -1830,80 +1840,98 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="22.75" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="24.75" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="D3" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="B11" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1913,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1955,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
> scoreboard structure create
</commit_message>
<xml_diff>
--- a/phonegap project.xlsx
+++ b/phonegap project.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\app\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="temp note" sheetId="2" r:id="rId1"/>
     <sheet name="APP idea" sheetId="3" r:id="rId2"/>
-    <sheet name="decision" sheetId="4" r:id="rId3"/>
-    <sheet name="scoreboard" sheetId="6" r:id="rId4"/>
-    <sheet name="vocabolary" sheetId="7" r:id="rId5"/>
-    <sheet name="close -&gt;" sheetId="5" r:id="rId6"/>
+    <sheet name="scoreboard" sheetId="6" r:id="rId3"/>
+    <sheet name="vocabolary" sheetId="7" r:id="rId4"/>
+    <sheet name="finish -&gt;" sheetId="5" r:id="rId5"/>
+    <sheet name="decision" sheetId="4" r:id="rId6"/>
     <sheet name="exercise" sheetId="1" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="219">
   <si>
     <t>clock centerlize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -654,10 +649,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>separate style.css</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>use localstorage replace mysql</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -701,7 +692,427 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>localstorage</t>
+    <t>show title, expand to list player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>how to prevent data been delete by other program =&gt; study phonegap DB plugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.toright.com/posts/2356/android-webapp-%E9%96%8B%E7%99%BC%E6%95%99%E5%AD%B8-html5-web-storage.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JavaScript Object Notation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0,4,5,2,7,8,3]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>phoneGap plugin study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APP alert/notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>一般函式轉換已包含</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>格式</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>物件(object)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>用大括號</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> { }</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"key":"value","score":80}, key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>一定要用文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>用數字需加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"")</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>陣列(array)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>用中括號</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> [ ]</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>物件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>陣列</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>損失</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>，只留下</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>陣列</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>物件</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>使用數字編碼</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>非英文要用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Unicode encode</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>                       [</t>
+  </si>
+  <si>
+    <t>                       ]   </t>
+  </si>
+  <si>
+    <t>                  }';</t>
+  </si>
+  <si>
+    <t>var obj = JSON.parse(json);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function Person( name, age, phone) {</t>
+  </si>
+  <si>
+    <t>                    this.name = name; </t>
+  </si>
+  <si>
+    <t>                    this.age = age; </t>
+  </si>
+  <si>
+    <t>                    this.phone = phone; </t>
+  </si>
+  <si>
+    <t>var person = new Person( "Roger", 30 , 0912345678); </t>
+  </si>
+  <si>
+    <t>json = person.toJSONString() ;</t>
+  </si>
+  <si>
+    <t>var object = JSON.parse(json);</t>
+  </si>
+  <si>
+    <t>Ex : object.person.name = Roger ; object.person.age = 30</t>
+  </si>
+  <si>
+    <t>JSON + localStorage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>                             {"player": "allen", "round": ["0","-10","50"] }, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>                             {"player": "andrew", "round": ["80","100","50"] }, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>var json = '{  "GameTitle"  : </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>建立物件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>將</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>字串轉為物件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>alert('I have ' + obj.GameTitle.length + ' cats.');    //</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>這裡會顯示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2 </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">alert(obj.GameTitle[0].player);     // </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>這裡會顯示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> allen</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -709,42 +1120,105 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>player_score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>allen!!-50!50!!200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>andrew!!100!-50!!80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oahehc_scoreboard_test_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oahehc_scoreboard_test_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>show title, expand to list player</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>how to prevent data been delete by other program =&gt; study phonegap DB plugin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://blog.toright.com/posts/2356/android-webapp-%E9%96%8B%E7%99%BC%E6%95%99%E5%AD%B8-html5-web-storage.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =&gt; use JSON for data?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">localStorage.removeItem("bar"); </t>
+    <t>Player1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player2</t>
+  </si>
+  <si>
+    <t>Player3</t>
+  </si>
+  <si>
+    <t>Player4</t>
+  </si>
+  <si>
+    <t>DB test form</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom function for JSON &lt;-&gt; localstorage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create title and player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title rename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>player delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>player add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>player rename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete -&gt; change to 0?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>form 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>form 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round2</t>
+  </si>
+  <si>
+    <t>round3</t>
+  </si>
+  <si>
+    <t>round4</t>
+  </si>
+  <si>
+    <t>checkbox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total amount auto check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score/money mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change page function design</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -755,7 +1229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="_-[$€]* #,##0.00_-;\-[$€]* #,##0.00_-;_-[$€]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -865,8 +1339,64 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -876,6 +1406,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8585"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,7 +1436,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -952,11 +1494,44 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,7 +1811,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1253,12 +1828,12 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="47.08984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="10"/>
-    <col min="3" max="3" width="54.6328125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="111.453125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="54.625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="111.5" style="10" customWidth="1"/>
     <col min="5" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
@@ -1373,7 +1948,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="68">
+    <row r="13" spans="1:4" ht="66">
       <c r="A13" s="11" t="s">
         <v>109</v>
       </c>
@@ -1416,7 +1991,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>42</v>
@@ -1427,7 +2002,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>51</v>
@@ -1436,7 +2011,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="85">
+    <row r="19" spans="1:4" ht="82.5">
       <c r="A19" s="14" t="s">
         <v>122</v>
       </c>
@@ -1447,9 +2022,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="34">
+    <row r="20" spans="1:4" ht="33">
       <c r="A20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>55</v>
@@ -1460,7 +2035,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>57</v>
@@ -1654,15 +2229,15 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1673,6 +2248,21 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1683,184 +2273,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="C2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7"/>
-      <c r="C3" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="15"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
-  <cols>
-    <col min="1" max="1" width="18.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="24.7265625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="2.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="56.625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1868,78 +2293,336 @@
       <c r="A1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>152</v>
+      <c r="D1" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5">
+      <c r="D4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5">
+      <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="D5" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="D4" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="D6" s="17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="17" t="s">
+    <row r="7" spans="1:5" ht="16.5">
+      <c r="A7" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5">
+      <c r="A8" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5">
+      <c r="A9" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>193</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="16.5">
+      <c r="A12" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:5" ht="16.5">
+      <c r="D19" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.5">
+      <c r="D20" s="27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5">
+      <c r="A21" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="D21" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" s="29"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="D32" s="29"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="D33" s="27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="7"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="7"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="28.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1948,36 +2631,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
-  <cols>
-    <col min="1" max="1" width="28.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
@@ -1988,10 +2641,175 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="25.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.75" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="C2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2003,12 +2821,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="1.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">

</xml_diff>